<commit_message>
work schedule update 2019.1.11
</commit_message>
<xml_diff>
--- a/workschedule.xlsx
+++ b/workschedule.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharmproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharm\tbeshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B549C764-699C-465A-ABE8-A1EBEC94C4A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="EB07" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1740" windowWidth="15480" windowHeight="9615"/>
+    <workbookView xWindow="420" yWindow="1740" windowWidth="15480" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="總表" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="工作成員名單">表2[工作成員名單]</definedName>
     <definedName name="具體任務名稱">表3[具體任務名稱]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -251,12 +252,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,7 +686,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="0" xr9:uid="{18F2F569-E11C-4E62-AE79-3C66A061B779}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -698,7 +701,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -776,7 +779,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -932,6 +934,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-02D4-4359-A30F-D6ABCD90EDF5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1017,10 +1024,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1094,6 +1101,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-02D4-4359-A30F-D6ABCD90EDF5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1179,10 +1191,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -1256,6 +1268,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-02D4-4359-A30F-D6ABCD90EDF5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1373,13 +1390,19 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="113" name="群組 112"/>
+        <xdr:cNvPr id="113" name="群組 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="228600" y="161925"/>
-          <a:ext cx="2590800" cy="1466849"/>
+          <a:ext cx="2590800" cy="1419224"/>
           <a:chOff x="1357290" y="2143116"/>
           <a:chExt cx="3676650" cy="2689225"/>
         </a:xfrm>
@@ -1393,7 +1416,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="114" name="AutoShape 3"/>
+          <xdr:cNvPr id="114" name="AutoShape 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
           </xdr:cNvSpPr>
@@ -1522,7 +1551,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="115" name="Freeform 6"/>
+          <xdr:cNvPr id="115" name="Freeform 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -2035,7 +2070,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="116" name="Freeform 7"/>
+          <xdr:cNvPr id="116" name="Freeform 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -2719,7 +2760,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="117" name="Freeform 8"/>
+          <xdr:cNvPr id="117" name="Freeform 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -3562,7 +3609,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="118" name="Freeform 9"/>
+          <xdr:cNvPr id="118" name="Freeform 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -4054,7 +4107,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="119" name="Freeform 10"/>
+          <xdr:cNvPr id="119" name="Freeform 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -4582,7 +4641,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="120" name="Freeform 11"/>
+          <xdr:cNvPr id="120" name="Freeform 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000078000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -5269,7 +5334,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="121" name="Freeform 12"/>
+          <xdr:cNvPr id="121" name="Freeform 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000079000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -5725,7 +5796,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="122" name="Freeform 13"/>
+          <xdr:cNvPr id="122" name="Freeform 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -6202,7 +6279,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="123" name="Freeform 14"/>
+          <xdr:cNvPr id="123" name="Freeform 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -6703,7 +6786,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="124" name="Freeform 15"/>
+          <xdr:cNvPr id="124" name="Freeform 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -7189,7 +7278,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="125" name="Freeform 16"/>
+          <xdr:cNvPr id="125" name="Freeform 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -7480,7 +7575,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="126" name="Freeform 17"/>
+          <xdr:cNvPr id="126" name="Freeform 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -7843,7 +7944,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="127" name="Freeform 18"/>
+          <xdr:cNvPr id="127" name="Freeform 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -8020,7 +8127,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="128" name="Freeform 19"/>
+          <xdr:cNvPr id="128" name="Freeform 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -8899,7 +9012,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="129" name="Freeform 20"/>
+          <xdr:cNvPr id="129" name="Freeform 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -9184,7 +9303,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="130" name="Freeform 21"/>
+          <xdr:cNvPr id="130" name="Freeform 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -10156,7 +10281,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="131" name="Freeform 22"/>
+          <xdr:cNvPr id="131" name="Freeform 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -11080,7 +11211,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="132" name="Freeform 23"/>
+          <xdr:cNvPr id="132" name="Freeform 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -11479,7 +11616,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="133" name="Freeform 24"/>
+          <xdr:cNvPr id="133" name="Freeform 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000085000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -11692,7 +11835,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="134" name="Freeform 25"/>
+          <xdr:cNvPr id="134" name="Freeform 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000086000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -11869,7 +12018,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="135" name="Freeform 26"/>
+          <xdr:cNvPr id="135" name="Freeform 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000087000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -12046,7 +12201,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="136" name="Freeform 27"/>
+          <xdr:cNvPr id="136" name="Freeform 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000088000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -12223,7 +12384,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="137" name="Freeform 28"/>
+          <xdr:cNvPr id="137" name="Freeform 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000089000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -13024,7 +13191,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="138" name="Freeform 29"/>
+          <xdr:cNvPr id="138" name="Freeform 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -13453,7 +13626,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="139" name="Freeform 30"/>
+          <xdr:cNvPr id="139" name="Freeform 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -14293,7 +14472,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="140" name="Freeform 31"/>
+          <xdr:cNvPr id="140" name="Freeform 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -14620,7 +14805,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="141" name="Freeform 32"/>
+          <xdr:cNvPr id="141" name="Freeform 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -15316,7 +15507,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="142" name="Freeform 33"/>
+          <xdr:cNvPr id="142" name="Freeform 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -16183,7 +16380,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="143" name="Freeform 34"/>
+          <xdr:cNvPr id="143" name="Freeform 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -16702,7 +16905,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="144" name="Freeform 35"/>
+          <xdr:cNvPr id="144" name="Freeform 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000090000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -17071,7 +17280,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="145" name="Freeform 36"/>
+          <xdr:cNvPr id="145" name="Freeform 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000091000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -17608,7 +17823,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="146" name="Freeform 37"/>
+          <xdr:cNvPr id="146" name="Freeform 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000092000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -18145,7 +18366,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="147" name="Freeform 38"/>
+          <xdr:cNvPr id="147" name="Freeform 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000093000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -18574,7 +18801,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="148" name="Freeform 39"/>
+          <xdr:cNvPr id="148" name="Freeform 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000094000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -19465,7 +19698,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="149" name="Freeform 40"/>
+          <xdr:cNvPr id="149" name="Freeform 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000095000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -20170,7 +20409,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="150" name="Freeform 41"/>
+          <xdr:cNvPr id="150" name="Freeform 41">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000096000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -20545,7 +20790,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="151" name="Freeform 42"/>
+          <xdr:cNvPr id="151" name="Freeform 42">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000097000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -21127,7 +21378,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="152" name="Freeform 43"/>
+          <xdr:cNvPr id="152" name="Freeform 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000098000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -21664,7 +21921,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="153" name="Freeform 44"/>
+          <xdr:cNvPr id="153" name="Freeform 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000099000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -22561,7 +22824,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="154" name="Freeform 45"/>
+          <xdr:cNvPr id="154" name="Freeform 45">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -23089,7 +23358,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="155" name="Freeform 46"/>
+          <xdr:cNvPr id="155" name="Freeform 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -23788,7 +24063,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="156" name="Freeform 47"/>
+          <xdr:cNvPr id="156" name="Freeform 47">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -24256,7 +24537,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="157" name="Freeform 48"/>
+          <xdr:cNvPr id="157" name="Freeform 48">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -25153,7 +25440,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="158" name="Freeform 49"/>
+          <xdr:cNvPr id="158" name="Freeform 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -25825,7 +26118,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="159" name="Freeform 50"/>
+          <xdr:cNvPr id="159" name="Freeform 50">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00009F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -26002,7 +26301,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="160" name="Freeform 51"/>
+          <xdr:cNvPr id="160" name="Freeform 51">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A0000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -27013,7 +27318,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="161" name="Freeform 52"/>
+          <xdr:cNvPr id="161" name="Freeform 52">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A1000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -27298,7 +27609,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="162" name="Freeform 53"/>
+          <xdr:cNvPr id="162" name="Freeform 53">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A2000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -27577,7 +27894,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="163" name="Freeform 54"/>
+          <xdr:cNvPr id="163" name="Freeform 54">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A3000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -28144,7 +28467,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="164" name="Freeform 55"/>
+          <xdr:cNvPr id="164" name="Freeform 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A4000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -28663,7 +28992,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="165" name="Freeform 56"/>
+          <xdr:cNvPr id="165" name="Freeform 56">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A5000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -28876,7 +29211,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="166" name="Freeform 57"/>
+          <xdr:cNvPr id="166" name="Freeform 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A6000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -29185,7 +29526,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="167" name="Freeform 58"/>
+          <xdr:cNvPr id="167" name="Freeform 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A7000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -29857,7 +30204,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="168" name="Freeform 59"/>
+          <xdr:cNvPr id="168" name="Freeform 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A8000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -30502,7 +30855,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="169" name="Freeform 60"/>
+          <xdr:cNvPr id="169" name="Freeform 60">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000A9000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -30907,7 +31266,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="170" name="Freeform 61"/>
+          <xdr:cNvPr id="170" name="Freeform 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AA000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -31144,7 +31509,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="171" name="Freeform 62"/>
+          <xdr:cNvPr id="171" name="Freeform 62">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AB000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -31519,7 +31890,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="172" name="Freeform 63"/>
+          <xdr:cNvPr id="172" name="Freeform 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AC000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -32653,7 +33030,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="173" name="Freeform 64"/>
+          <xdr:cNvPr id="173" name="Freeform 64">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AD000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -33700,7 +34083,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="174" name="Freeform 65"/>
+          <xdr:cNvPr id="174" name="Freeform 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AE000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -34165,7 +34554,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="175" name="Freeform 66"/>
+          <xdr:cNvPr id="175" name="Freeform 66">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AF000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -34993,7 +35388,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="176" name="Freeform 67"/>
+          <xdr:cNvPr id="176" name="Freeform 67">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B0000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -35578,7 +35979,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="177" name="Freeform 68"/>
+          <xdr:cNvPr id="177" name="Freeform 68">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B1000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -35899,7 +36306,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="178" name="Freeform 69"/>
+          <xdr:cNvPr id="178" name="Freeform 69">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B2000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -36580,7 +36993,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="179" name="Freeform 70"/>
+          <xdr:cNvPr id="179" name="Freeform 70">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B3000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -36955,7 +37374,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="180" name="Freeform 71"/>
+          <xdr:cNvPr id="180" name="Freeform 71">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B4000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -37768,7 +38193,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="181" name="Freeform 72"/>
+          <xdr:cNvPr id="181" name="Freeform 72">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B5000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -38389,7 +38820,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="182" name="Freeform 73"/>
+          <xdr:cNvPr id="182" name="Freeform 73">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B6000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -39226,7 +39663,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="183" name="Freeform 74"/>
+          <xdr:cNvPr id="183" name="Freeform 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B7000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -40015,7 +40458,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="184" name="Freeform 75"/>
+          <xdr:cNvPr id="184" name="Freeform 75">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B8000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -40252,7 +40701,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="185" name="Freeform 76"/>
+          <xdr:cNvPr id="185" name="Freeform 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000B9000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -40741,7 +41196,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="186" name="Freeform 77"/>
+          <xdr:cNvPr id="186" name="Freeform 77">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BA000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -41242,7 +41703,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="187" name="Freeform 78"/>
+          <xdr:cNvPr id="187" name="Freeform 78">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BB000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -41737,7 +42204,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="188" name="Freeform 79"/>
+          <xdr:cNvPr id="188" name="Freeform 79">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BC000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -42028,7 +42501,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="189" name="Freeform 80"/>
+          <xdr:cNvPr id="189" name="Freeform 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BD000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -42391,7 +42870,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="190" name="Freeform 81"/>
+          <xdr:cNvPr id="190" name="Freeform 81">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BE000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -42568,7 +43053,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="191" name="Freeform 82"/>
+          <xdr:cNvPr id="191" name="Freeform 82">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BF000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -43462,7 +43953,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="192" name="Freeform 83"/>
+          <xdr:cNvPr id="192" name="Freeform 83">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C0000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -44254,7 +44751,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="193" name="Freeform 84"/>
+          <xdr:cNvPr id="193" name="Freeform 84">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C1000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -44551,7 +45054,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="194" name="Freeform 85"/>
+          <xdr:cNvPr id="194" name="Freeform 85">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C2000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -45538,7 +46047,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="195" name="Freeform 86"/>
+          <xdr:cNvPr id="195" name="Freeform 86">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C3000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -45715,7 +46230,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="196" name="Freeform 87"/>
+          <xdr:cNvPr id="196" name="Freeform 87">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C4000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -46018,7 +46539,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="197" name="Freeform 88"/>
+          <xdr:cNvPr id="197" name="Freeform 88">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C5000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -46885,7 +47412,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="198" name="Freeform 89"/>
+          <xdr:cNvPr id="198" name="Freeform 89">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C6000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -47218,7 +47751,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="199" name="Freeform 90"/>
+          <xdr:cNvPr id="199" name="Freeform 90">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C7000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -47395,7 +47934,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="200" name="Freeform 91"/>
+          <xdr:cNvPr id="200" name="Freeform 91">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C8000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -47572,7 +48117,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="201" name="Freeform 92"/>
+          <xdr:cNvPr id="201" name="Freeform 92">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000C9000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -48529,7 +49080,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="202" name="Freeform 93"/>
+          <xdr:cNvPr id="202" name="Freeform 93">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CA000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -48706,7 +49263,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="203" name="Freeform 94"/>
+          <xdr:cNvPr id="203" name="Freeform 94">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CB000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -49486,7 +50049,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="204" name="Freeform 95"/>
+          <xdr:cNvPr id="204" name="Freeform 95">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CC000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -50764,7 +51333,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="205" name="Freeform 96"/>
+          <xdr:cNvPr id="205" name="Freeform 96">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CD000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -51181,7 +51756,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="206" name="Freeform 97"/>
+          <xdr:cNvPr id="206" name="Freeform 97">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CE000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -51358,7 +51939,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="207" name="Freeform 98"/>
+          <xdr:cNvPr id="207" name="Freeform 98">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CF000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -51769,7 +52356,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="208" name="Freeform 99"/>
+          <xdr:cNvPr id="208" name="Freeform 99">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D0000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -51994,7 +52587,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="209" name="Freeform 100"/>
+          <xdr:cNvPr id="209" name="Freeform 100">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D1000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -52171,7 +52770,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="210" name="Freeform 101"/>
+          <xdr:cNvPr id="210" name="Freeform 101">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D2000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -52348,7 +52953,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="211" name="Freeform 102"/>
+          <xdr:cNvPr id="211" name="Freeform 102">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D3000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -52525,7 +53136,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="212" name="Freeform 103"/>
+          <xdr:cNvPr id="212" name="Freeform 103">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D4000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -52798,7 +53415,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="213" name="Freeform 104"/>
+          <xdr:cNvPr id="213" name="Freeform 104">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D5000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks/>
           </xdr:cNvSpPr>
@@ -53089,6 +53712,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="214" name="圓角矩形 213">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D6000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -53152,6 +53780,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="215" name="圓角矩形 214">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D7000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -53209,10 +53842,6 @@
             <a:rPr lang="zh-TW" altLang="en-US" sz="1400"/>
             <a:t>任務</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-TW" sz="1400"/>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="zh-TW" sz="1400"/>
           </a:br>
@@ -53245,7 +53874,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="图表 8"/>
+        <xdr:cNvPr id="9" name="图表 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -53277,6 +53912,11 @@
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="13" name="群組 12">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
@@ -53290,7 +53930,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="動作按鈕: 首頁 13"/>
+          <xdr:cNvPr id="14" name="動作按鈕: 首頁 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -53446,7 +54092,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="文字方塊 14"/>
+          <xdr:cNvPr id="15" name="文字方塊 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -53519,6 +54171,11 @@
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="11" name="群組 10">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
@@ -53532,7 +54189,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="動作按鈕: 首頁 8"/>
+          <xdr:cNvPr id="9" name="動作按鈕: 首頁 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -53690,6 +54353,11 @@
         <xdr:nvSpPr>
           <xdr:cNvPr id="10" name="文字方塊 9">
             <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+              </a:ext>
+            </a:extLst>
           </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
@@ -53745,18 +54413,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B8:H33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B8:H33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="B8:H33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B8:H33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="員工姓名" dataDxfId="6"/>
-    <tableColumn id="2" name="任務名稱" dataDxfId="5"/>
-    <tableColumn id="3" name="開始時間" dataDxfId="4"/>
-    <tableColumn id="4" name="結束時間" dataDxfId="3"/>
-    <tableColumn id="5" name="已完成(%)" dataDxfId="2"/>
-    <tableColumn id="6" name="所需總天數" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="員工姓名" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="任務名稱" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="開始時間" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="結束時間" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="已完成(%)" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="所需總天數" dataDxfId="1">
       <calculatedColumnFormula>IF(F9="",0,(E9-D9+1)*F9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="還需工作日(天)" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="還需工作日(天)" dataDxfId="0">
       <calculatedColumnFormula>E9-D9+1-G9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -53765,25 +54433,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:A14" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表2" displayName="表2" ref="A3:A14" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" name="工作成員名單"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="工作成員名單"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="C3:C22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表3" displayName="表3" ref="C3:C22" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" name="具體任務名稱"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="具體任務名稱"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -53858,6 +54526,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -53893,6 +54578,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -54068,14 +54770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="17.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" style="1" customWidth="1"/>
@@ -54088,16 +54790,16 @@
     <col min="9" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:8" ht="30.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" ht="9.75" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:8" ht="27" thickTop="1" thickBot="1">
       <c r="D2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="2:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:8" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" ht="24.75" customHeight="1" thickBot="1"/>
+    <row r="4" spans="2:8" ht="27.75" customHeight="1" thickTop="1">
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
@@ -54106,7 +54808,7 @@
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="27.75" customHeight="1">
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
@@ -54115,7 +54817,7 @@
       </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="2:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="27.75" customHeight="1" thickBot="1">
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
@@ -54124,12 +54826,12 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:8" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="24" customHeight="1" thickTop="1">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8">
       <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
@@ -54152,7 +54854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="24.75" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
@@ -54166,18 +54868,18 @@
         <v>43474</v>
       </c>
       <c r="F9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" ref="G9:G33" si="0">IF(F9="",0,(E9-D9+1)*F9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" ref="H9:H33" si="1">E9-D9+1-G9</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="24.75" customHeight="1">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
@@ -54191,18 +54893,18 @@
         <v>43476</v>
       </c>
       <c r="F10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="24.75" customHeight="1">
       <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
@@ -54227,7 +54929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="24.75" customHeight="1">
       <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
@@ -54252,7 +54954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="24.75" customHeight="1">
       <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
@@ -54277,7 +54979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" ht="24.75" customHeight="1">
       <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
@@ -54302,7 +55004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" ht="24.75" customHeight="1">
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -54327,7 +55029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8" ht="24.75" customHeight="1">
       <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
@@ -54352,7 +55054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" ht="24.75" customHeight="1">
       <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
@@ -54377,7 +55079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" ht="24.75" customHeight="1">
       <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
@@ -54402,7 +55104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:8" ht="24.75" customHeight="1">
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
@@ -54427,7 +55129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:8" ht="24.75" customHeight="1">
       <c r="B20" s="7" t="s">
         <v>16</v>
       </c>
@@ -54452,7 +55154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:8" ht="24.75" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>16</v>
       </c>
@@ -54477,7 +55179,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:8" ht="24.75" customHeight="1">
       <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
@@ -54502,7 +55204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:8" ht="24.75" customHeight="1">
       <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
@@ -54527,7 +55229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8" ht="24.75" customHeight="1">
       <c r="B24" s="7" t="s">
         <v>16</v>
       </c>
@@ -54552,7 +55254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:8" ht="24.75" customHeight="1">
       <c r="B25" s="7" t="s">
         <v>16</v>
       </c>
@@ -54577,7 +55279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:8" ht="24.75" customHeight="1">
       <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
@@ -54602,7 +55304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:8" ht="24.75" customHeight="1">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
@@ -54617,7 +55319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:8" ht="24.75" customHeight="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
@@ -54632,7 +55334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:8" ht="24.75" customHeight="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
@@ -54647,7 +55349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:8" ht="24.75" customHeight="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
@@ -54662,7 +55364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:8" ht="24.75" customHeight="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
@@ -54677,7 +55379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:8" ht="24.75" customHeight="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
@@ -54692,7 +55394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:8" ht="24.75" customHeight="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -54738,10 +55440,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>工作成員名單</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C33" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>具體任務名稱</formula1>
     </dataValidation>
   </dataValidations>
@@ -54755,12 +55457,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <sheetProtection password="EB07" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -54771,27 +55473,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="3" max="3" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="22.5">
       <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -54799,7 +55501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -54807,7 +55509,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -54815,7 +55517,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -54823,73 +55525,73 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3">
       <c r="C7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3">
       <c r="C8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="A9" s="10"/>
       <c r="C9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3">
       <c r="A10" s="10"/>
       <c r="C10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" s="10"/>
       <c r="C11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3">
       <c r="A12" s="10"/>
       <c r="C12" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3">
       <c r="A13" s="10"/>
       <c r="C13" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3">
       <c r="A14" s="10"/>
       <c r="C14" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3">
       <c r="C15" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3">
       <c r="C16" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:3">
       <c r="C17" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:3">
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:3">
       <c r="C19" t="s">
         <v>57</v>
       </c>

</xml_diff>